<commit_message>
fix: spatial info scraping
</commit_message>
<xml_diff>
--- a/output/planilhas/leilaoimoveis_aquiraz-ce.xlsx
+++ b/output/planilhas/leilaoimoveis_aquiraz-ce.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,77 +543,57 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>176124</v>
-      </c>
-      <c r="C2" t="n">
-        <v>168</v>
-      </c>
-      <c r="D2" t="n">
-        <v>73.52</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10.800,00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>176124</v>
-      </c>
-      <c r="H2" t="n">
-        <v>134742.91</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>23.49542935658967</v>
+        <v>0</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>13/05/2024</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>22/05/2024</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Leilão SFI Caixa</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Leilão Caixa </t>
-        </is>
-      </c>
+          <t>Venda Direta Caixa</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
-          <t>26700</t>
+          <t>13760</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>1123127</t>
+          <t>65111</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>RUA ALDEMIR MARTINS,N. 734, TABAJARA - CEP: 61700-000, AQUIRAZ - CEARA</t>
+          <t>AVENIDA 01,N. 00 QD 31, LTS 1-15 E 26-40, LAGOA DO PATANHÉM - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-rotta-del-mar-2-quartos-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1625939-8444423002750-venda-direta-caixa</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lagoa-do-patanhem-existe-indisponibilidade-gravada-nos-av-07-av-08-av-09-av-10-a-imovel-caixa-economica-federal-cef-1992372-10197066-venda-direta-caixa</t>
         </is>
       </c>
     </row>
@@ -623,23 +603,23 @@
           <t>Casa</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>145000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>216</v>
-      </c>
-      <c r="D3" t="n">
-        <v>75</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>186,96</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>135,55</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>145000</v>
-      </c>
-      <c r="H3" t="n">
-        <v>204917.99</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
@@ -647,48 +627,36 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>14/02/2024</t>
+          <t>13/08/2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>02/04/2024</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>11/04/2024</t>
-        </is>
-      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Leilão SFI Caixa</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Leilão Caixa </t>
-        </is>
-      </c>
+          <t>Venda Direta Caixa</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>21087</t>
+          <t>22906</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>111226</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>RUA A N 10,N. 10, CENTRO - CEP: 61700-000, AQUIRAZ - CEARA</t>
+          <t>RUA 18,N. 1843 QD F LT 3, PRAINHA - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-pq-entre-praias-imovel-caixa-economica-federal-cef-1600178-8444407824384-venda-direta-caixa</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-prainha-3-quartos-1-vaga-na-garagem-area-de-servico-imovel-caixa-economica-federal-cef-1862019-1444417428360-venda-direta-caixa</t>
         </is>
       </c>
     </row>
@@ -698,86 +666,79 @@
           <t>Casa</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>627130</v>
-      </c>
-      <c r="C4" t="n">
-        <v>462</v>
-      </c>
-      <c r="D4" t="n">
-        <v>189.66</v>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>77,00</t>
+        </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="n">
         <v>2</v>
       </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>850000</v>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>26.22</v>
+        <v>0</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>16/02/2023</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>14/03/2024</t>
-        </is>
-      </c>
+          <t>28/03/2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Venda Online Caixa</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
-</t>
-        </is>
-      </c>
+          <t>Venda Direta Caixa</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
-          <t>19354</t>
+          <t>4810</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>0101180038000002</t>
+          <t>112278</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>AVENIDA LITORANEA,N. 5297 CS 01, PORTO DAS DUNAS - CEP: 61700-000, AQUIRAZ - CEARA</t>
+          <t>RUA ERNESTO BENTO DE FREITAS,N. 856 CS 13, PAV TERREO, DISTRITO DE ITAPERA - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-cond-porto-riviera-3-quartos-2-vagas-na-garagem-varanda-sacada-area-de-se-imovel-caixa-economica-federal-cef-1218909-1555512336347-venda-direta-caixa</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-cond-vila-jatoba-02-2-quartos-1-vaga-na-garagem-varanda-sacada-wc-sala-imovel-caixa-economica-federal-cef-1660428-8555535488656-venda-direta-caixa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>390080</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>213,60</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>189,66</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -788,7 +749,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>21/03/2025</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
@@ -796,22 +757,32 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="n">
-        <v>0</v>
+          <t>Leilão SFI Caixa</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Só Leilões </t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>19384</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE B44, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>AVENIDA LITORÂNEA,N. 5297 CS 02, PARTE A - IV ETAPA, PORTO DAS DUNAS - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176567-desocupado-imovel-1291388</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-acj-construtora-e-incorporadora-ltda-3-quartos-2-vagas-na-garagem-area-de-imovel-caixa-economica-federal-cef-2185568-1555513592835-venda-direta-caixa</t>
         </is>
       </c>
     </row>
@@ -821,10 +792,12 @@
           <t>Terreno</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>414460</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.113,70</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -837,7 +810,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>13/08/2024</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
@@ -845,37 +818,51 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
+          <t>Venda Direta Caixa</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="n">
-        <v>0</v>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>17146</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE F29, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>VIA COLETORA DE CONTORNO I,N. 00 QD 8, LT 10-11, MARIUBA, PORTO DAS DUNAS II - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176568-desocupado-imovel-1291387</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-porto-das-dunas-ii-imovel-caixa-economica-federal-cef-1862020-10190921-venda-direta-caixa</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>950820</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>220,91</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>194,33</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -886,7 +873,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>11/02/2024</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
@@ -904,25 +891,27 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE D69/D82, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>RUA LAIS SIDRIM TARGINO, S/N, QUADRA 13, APTO DUPLEX C-02, BLOCO J, CONDOMÍNIO VILA DO PORTO RESORT, GRAIA, AQUIRAZ, CE, 61700-000</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176569-desocupado-imovel-1291386</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-apartamento-residencial-graia-4-dormitorio-s-3-vaga-s-de-garagem-desocupado-imovel-1598512</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>451030</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5.216,10</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -935,7 +924,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>06/03/2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
@@ -943,37 +932,49 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr"/>
+          <t>Judicial</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nasar Leilões </t>
+        </is>
+      </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE D49, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>RUA CLOVES HOLANDA DE FREITAS</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176570-desocupado-imovel-1291384</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-01-um-terreno-situado-no-lugar-pau-pombo-distrito-de-tapera-desta-comarca-localizado-a-rua-clov-imovel-2168227</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>426650</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>180,00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>67,34</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -984,7 +985,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>22/02/2025</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -992,37 +993,55 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="n">
-        <v>0</v>
+          <t>Leilão SFI Caixa</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leffa Leilões </t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>19059</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0000</t>
+        </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE D100, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>RUA B,N. 377 ATUAL RUA WALDIR MEDEIROS DA SILVA, CABECEIRA DA ROÇA - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176571-desocupado-imovel-1291383</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-lot-brisa-das-praias-2-quartos-area-de-servico-wc-sala-cozinha-terraco-imovel-caixa-economica-federal-cef-2153548-8555514750254-venda-direta-caixa</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>414460</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>198,00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>92,40</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -1033,7 +1052,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>07/01/2025</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
@@ -1041,38 +1060,56 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="n">
-        <v>0</v>
+          <t>Licitação Aberta Caixa</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Joyce Ribeiro Leilões </t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>23452</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0000110973</t>
+        </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE D30, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>RUA ARTEMISIA,N. 457 TERRENO 01 PARTE LT 22 QD S, SANTA MARIA - CEP: 61700-000, AQUIRAZ - CEARA</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176572-desocupado-imovel-1291382</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-lot-parque-das-flores-3-quartos-1-vaga-na-garagem-area-de-servico-2-wc-s-imovel-caixa-economica-federal-cef-2086542-8444415785619-venda-direta-caixa</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>487600</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>525,00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>336,00</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
@@ -1082,7 +1119,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>29/04/2023</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="M11" t="inlineStr"/>
@@ -1090,54 +1127,54 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr"/>
+          <t>Extrajudicial</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mega Leilões </t>
+        </is>
+      </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
         <v>0</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>RUA UM, S/N, ENSEADA PRAIA, LOTE D103, CONDOMÍNIO AQUIRAZ RIVIERA, CURRALINHO, AQUIRAZ, CE, 61700-000</t>
+          <t>RUA TAINHA, 92, MARIUBA, AQUIRAZ, CE</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-lote-residencial-curralinho-idr176573-desocupado-imovel-1291381</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-casa-336-m-mariuba-aquiraz-ce-desocupado-imovel-banco-santander-2182234</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>155665</v>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="n">
-        <v>92.84999999999999</v>
-      </c>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2.500,00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
-        <v>179000</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>13.03631284916201</v>
+        <v>0</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/03/2025</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1145,43 +1182,45 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr"/>
+          <t>Judicial</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nasar Leilões </t>
+        </is>
+      </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
         <v>0</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>RUA C, 55, PARQUE DA PRAINHA, AQUIRAZ, CE, 61700-000</t>
+          <t>RUA DAS SARDINHAS, 3214, PORTO DAS DUNAS</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-casa-residencial-parque-da-prainha-3-dormitorio-s-2-vaga-s-de-garagem-idr177409-imovel-1551713</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-matricula-do-imovel-n-22-849-cartorio-florencio-aquiraz-ce-cnm-019356-2-0022849-84-um-imovel-2168218</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Apartamento</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>810000</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>442,35</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>3</v>
-      </c>
-      <c r="G13" t="n">
-        <v>810000</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1190,15 +1229,11 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>07/03/2024</t>
+          <t>14/03/2025</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>20/03/2024</t>
-        </is>
-      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
@@ -1207,7 +1242,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Sato Leilões </t>
+          <t xml:space="preserve"> Biasi Leilões </t>
         </is>
       </c>
       <c r="R13" t="inlineStr"/>
@@ -1216,12 +1251,12 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>RUA LAIS SIDRIM TARGINO, S/N, QUADRA 13, APTO DUPLEX C-02, BLOCO J, CONDOMÍNIO VILA DO PORTO RESORT, GRAIA, AQUIRAZ, CE, 61700-000</t>
+          <t>ALAMEDA ANTURIUS, RESERVA TERRA BRASILIS - JACUNDÁ, AQUIRAZ/CE</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-apartamento-graia-aquiraz-ce-desocupado-imovel-1628765</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-terreno-no-loteamento-reserva-terra-brasilis-b-aquiraz-ce-imovel-2178006</t>
         </is>
       </c>
     </row>
@@ -1231,18 +1266,16 @@
           <t>Apartamento</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>2250000</v>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
-        <v>203</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2,54</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
-        <v>2250000</v>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
@@ -1251,24 +1284,20 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>06/03/2024</t>
+          <t>14/03/2025</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>22/03/2024</t>
-        </is>
-      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Extrajudicial</t>
+          <t>Judicial</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Montenegro Leilões </t>
+          <t xml:space="preserve"> Taba Leilões </t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1277,36 +1306,32 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>AV. MARGINAL, LOTE A13/A14, TAPERA, AQUIRAZ/CE</t>
+          <t>RUA 10, AQUIRAZ - CE</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-ap-302-bg-21-manhattan-beach-riviera-imovel-1625677</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-aquiraz-ce-aquiraz-riviera-terreno-d-69-82-cod-do-leilao-e172-002-residenciais-imovel-2176521</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>368000</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>224.75</v>
-      </c>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1,12</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>368000</v>
-      </c>
-      <c r="H15" t="n">
-        <v>484555.91</v>
-      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
@@ -1314,97 +1339,75 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>27/02/2024</t>
+          <t>14/03/2025</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>22/04/2024</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>03/05/2024</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Leilão SFI Caixa</t>
+          <t>Judicial</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ARG Leilões </t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>3832</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>39571</t>
-        </is>
+          <t xml:space="preserve"> Taba Leilões </t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="n">
+        <v>0</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>RUA 5 SN PLANALTO DO SOL LOTES 06 07 24 E 25 QUADR,N. SN LTS 06 07 24 E 25- PLANALTO DO SOL</t>
+          <t>RUA 14, AQUIRAZ - CE</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-casa-imovel-caixa-economica-federal-cef-1612271</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-aquiraz-ce-aquiraz-riviera-terreno-d-49-cod-do-leilao-e172-003-residenciais-imovel-2176520</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>188100</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>130.91</v>
-      </c>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1,27</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>188100</v>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>300000</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
-        <v>37.3</v>
+        <v>0</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>27/02/2024</t>
+          <t>14/03/2025</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>18/03/2024</t>
-        </is>
-      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Extrajudicial</t>
+          <t>Judicial</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mega Leilões </t>
+          <t xml:space="preserve"> Taba Leilões </t>
         </is>
       </c>
       <c r="R16" t="inlineStr"/>
@@ -1413,35 +1416,27 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>RUA D, 38, BRISAS DAS PRAIAS, AQUIRAZ, CE</t>
+          <t>RUA 16, AQUIRAZ - CE</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-casa-130-m-brisas-das-praias-aquiraz-ce-desocupado-imovel-banco-santander-1615126</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-aquiraz-ce-aquiraz-riviera-terreno-d-103-cod-do-leilao-e172-016-residenciais-imovel-2176506</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>512639.47</v>
-      </c>
+          <t>Outros</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>4</v>
-      </c>
-      <c r="F17" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" t="n">
-        <v>512639.47</v>
-      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -1450,382 +1445,34 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>03/02/2024</t>
+          <t>15/01/2025</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>22/03/2024</t>
-        </is>
-      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Leilão SFI Caixa</t>
+          <t>Judicial</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Leilões Ceruli </t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>16856</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t xml:space="preserve"> Pereira Leilões </t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="n">
+        <v>0</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>RUA VIA LOCAL 35, SN- PARTE DO LT 01 QD 62</t>
+          <t>LOTEAMENTO AQUIRAZ RIVIERA</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-imovel-residencial-em-aquiraz-ce-imovel-caixa-economica-federal-cef-1588792</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Apartamento</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>96000</v>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>96000</v>
-      </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>30/10/2021</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>12/11/2021</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Graça Medeiros Leilões </t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>LOTEAMENTO ROTA DEL MAR</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/residencial-apartamento-empreendimento-residencial-saint-germain-aquiraz-ce-imovel-837788</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>204000</v>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="n">
-        <v>204000</v>
-      </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>14/10/2023</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>10/11/2023</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Graça Medeiros Leilões </t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-imovel-imovel-1484166</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Área Rural</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>15000</v>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="n">
-        <v>15000</v>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>14/10/2023</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>10/11/2023</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Graça Medeiros Leilões </t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/rural-imovel-imovel-1484147</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Outros</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>2745000</v>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>2745000</v>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>14/10/2023</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>10/11/2023</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Graça Medeiros Leilões </t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/outros-imovel-imovel-1484142</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Comercial</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>90000</v>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>90000</v>
-      </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>14/10/2023</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>10/11/2023</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Graça Medeiros Leilões </t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/comercial-imovel-imovel-1484131</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>60000</v>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>60000</v>
-      </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>30/10/2021</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>12/11/2021</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>Venda Direta</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Graça Medeiros Leilões </t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>SITUADO NO LUGAR DENOMINADO PUCABA, ANTIGO DISTRITO DE EUSÉBIO, AQUIRAZ – CE, HOJE MUNICÍPIO DE EUSÉBIO / CE, DENOMINADO “ PARQUE BRISA-MAR”</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/terreno-terreno-em-aquiraz-ce-imovel-837793</t>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/aquiraz/outros-imovel-no-loteamento-aquiraz-riviera-com-1-544-88m-imovel-2096382</t>
         </is>
       </c>
     </row>

</xml_diff>